<commit_message>
Removed the unnecessary 'Category' column from Code Review Part I
</commit_message>
<xml_diff>
--- a/Documents/Code Review Part I.xlsx
+++ b/Documents/Code Review Part I.xlsx
@@ -24,63 +24,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Code Styling </t>
   </si>
   <si>
-    <t>Checklist Item</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>Well-Documented Code</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Well-Documented Files</t>
   </si>
   <si>
     <t>Conventional and Relevant Names</t>
   </si>
   <si>
-    <t>Names</t>
-  </si>
-  <si>
     <t>No Similar Names</t>
   </si>
   <si>
     <t>Minimize Duplicated Code</t>
   </si>
   <si>
-    <t>Functions</t>
-  </si>
-  <si>
     <t>Small and Easy-to-Understand Functions</t>
   </si>
   <si>
     <t>Small and Easy-to-Understand Classes</t>
   </si>
   <si>
-    <t>Classes</t>
-  </si>
-  <si>
     <t>Security</t>
   </si>
   <si>
     <t>No Global Variables</t>
   </si>
   <si>
-    <t>Basics</t>
-  </si>
-  <si>
     <t>Code, Class, and Function Organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basics </t>
   </si>
   <si>
     <t>Documentation on Security Concerns/Information</t>
@@ -102,7 +78,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +100,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,60 +129,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -325,70 +265,54 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -399,6 +323,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,317 +614,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="14" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="2" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="2" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="25">
+        <v>43951</v>
+      </c>
+      <c r="E15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9">
-        <v>43951</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:F17"/>
+  <mergeCells count="16">
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>